<commit_message>
actualizacion en cesantias enero 2015
actualizacion en reportes de liquidacion de cesantias
</commit_message>
<xml_diff>
--- a/TotalPlano.xlsx
+++ b/TotalPlano.xlsx
@@ -5958,7 +5958,7 @@
         <v>213</v>
       </c>
       <c r="D241" s="1">
-        <v>256800008227</v>
+        <v>256800036996</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -6684,7 +6684,7 @@
         <v>258</v>
       </c>
       <c r="D293" s="1">
-        <v>0</v>
+        <v>256700068933</v>
       </c>
     </row>
     <row r="294" spans="1:4">
@@ -6754,7 +6754,7 @@
         <v>263</v>
       </c>
       <c r="D298" s="1">
-        <v>0</v>
+        <v>236000686170</v>
       </c>
     </row>
     <row r="299" spans="1:4">
@@ -6880,7 +6880,7 @@
         <v>272</v>
       </c>
       <c r="D307" s="1">
-        <v>0</v>
+        <v>256700043035</v>
       </c>
     </row>
     <row r="308" spans="1:4">
@@ -7538,7 +7538,7 @@
         <v>316</v>
       </c>
       <c r="D354" s="1">
-        <v>0</v>
+        <v>236800024473</v>
       </c>
     </row>
     <row r="355" spans="1:4">
@@ -9484,7 +9484,7 @@
         <v>444</v>
       </c>
       <c r="D493" s="1">
-        <v>236870037578</v>
+        <v>236870037579</v>
       </c>
     </row>
     <row r="494" spans="1:4">
@@ -12242,7 +12242,7 @@
         <v>621</v>
       </c>
       <c r="D690" s="1">
-        <v>0</v>
+        <v>236070198254</v>
       </c>
     </row>
     <row r="691" spans="1:4">

</xml_diff>